<commit_message>
worked on aufgabe 5 dokumentation
</commit_message>
<xml_diff>
--- a/pivot.xlsx
+++ b/pivot.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucaa\Documents\TBZ\M104\06_lb2\data_warehousing_carl_luca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucaa\Documents\TBZ\M104\06_lb2\data_warehousing_carl_luca\m104-data-warehousing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA6C8A0-9248-48C4-B397-E56F4D7A803F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2D42AA-3786-41A0-AB55-C9F88108A3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{440B290F-B62C-4737-B7EE-64C3CDBCCF03}"/>
   </bookViews>
@@ -20,8 +20,8 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="6" r:id="rId5"/>
-    <pivotCache cacheId="9" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -175,9 +175,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -197,6 +196,1531 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[pivot.xlsx]Sheet2!PivotTable3</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$8:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Damenschuhe</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$10:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bremen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dortmund</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Essen</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Frankfurt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hamburg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Koeln</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$10:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9213.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9528.76</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6221.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8780.630000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6615.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8386.89</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-26E6-4C33-A360-D654A2AA1BEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$8:$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Herrenschuhe</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$10:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bremen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dortmund</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Essen</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Frankfurt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hamburg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Koeln</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$10:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6468.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6184.1799999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7793.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5426.95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5994.8799999999992</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5837.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-26E6-4C33-A360-D654A2AA1BEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$8:$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kinderschuhe</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$10:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bremen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dortmund</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Essen</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Frankfurt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hamburg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Koeln</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$10:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4462.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4704.1400000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4792.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4154.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3758.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4264.51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-26E6-4C33-A360-D654A2AA1BEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$8:$E$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pflegemittel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$10:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bremen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dortmund</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Essen</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Frankfurt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hamburg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Koeln</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$10:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3727.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4050</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3817.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3712.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3847.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-26E6-4C33-A360-D654A2AA1BEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$8:$F$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Zubehoer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$10:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Bremen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dortmund</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Essen</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Frankfurt</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Hamburg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Koeln</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$10:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2690.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2895.1099999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2878.53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2646.4900000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2900.64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2922.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-26E6-4C33-A360-D654A2AA1BEA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="895970591"/>
+        <c:axId val="1746989471"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="895970591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1746989471"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1746989471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="895970591"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{772E11ED-3DD8-C9D5-E30D-2119B3C096AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3623,7 +5147,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{293687DA-2C9D-44B1-9883-C2FD4F330CF6}" name="PivotTable3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{293687DA-2C9D-44B1-9883-C2FD4F330CF6}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="A8:G16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" showAll="0">
@@ -3772,6 +5296,68 @@
   <dataFields count="1">
     <dataField name="Sum of Gewinn" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -3785,7 +5371,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FAA4317D-9E24-4D41-83F3-67920E7AEF33}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FAA4317D-9E24-4D41-83F3-67920E7AEF33}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C4" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="3">
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -4258,8 +5844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA108378-64A6-4E6B-8678-ECC5B25B3C69}">
   <dimension ref="A3:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4285,18 +5871,18 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>9775</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>152681.70000000001</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>411880.7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -4304,15 +5890,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
@@ -4335,168 +5921,169 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>9213.76</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>6468.16</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>4462.34</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
         <v>3727.5</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>2690.69</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <v>26562.45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>9528.76</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>6184.1799999999994</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>4704.1400000000003</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
         <v>4050</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
         <v>2895.1099999999997</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11">
         <v>27362.19</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>6221.25</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>7793.33</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>4792.08</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
         <v>3817.5</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
         <v>2878.53</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12">
         <v>25502.69</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>8780.630000000001</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>5426.95</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>4154.59</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>4005</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>2646.4900000000002</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13">
         <v>25013.660000000003</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>6615.01</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>5994.8799999999992</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>3758.92</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
         <v>3712.5</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>2900.64</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14">
         <v>22981.949999999997</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>8386.89</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>5837.12</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>4264.51</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
         <v>3847.5</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>2922.74</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15">
         <v>25258.759999999995</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>48746.3</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>37704.620000000003</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>26136.58</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
         <v>23160</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>16934.199999999997</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16">
         <v>152681.70000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changed Pivot table to include graph
</commit_message>
<xml_diff>
--- a/pivot.xlsx
+++ b/pivot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucaa\Documents\TBZ\M104\06_lb2\data_warehousing_carl_luca\m104-data-warehousing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2D42AA-3786-41A0-AB55-C9F88108A3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4751ADD8-C29E-4661-9B46-7E087B957179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{440B290F-B62C-4737-B7EE-64C3CDBCCF03}"/>
   </bookViews>
@@ -5845,7 +5845,7 @@
   <dimension ref="A3:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>